<commit_message>
Implemented basic obstacle avoidance. Using inverse proximity vector.
</commit_message>
<xml_diff>
--- a/Design/Mechanical/Inertia Calculation/Bifilar pendulum test 1.xlsx
+++ b/Design/Mechanical/Inertia Calculation/Bifilar pendulum test 1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GusBus\Documents\Masters\Matlab\Bifilar Pendulum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GusBus\Documents\Masters\Design\Mechanical\Inertia Calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,6 +601,10 @@
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>_xlfn.STDEV.S(E4:E12)</f>
+        <v>1.0638423828562688E-3</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
         <v>0.16939619436602332</v>
@@ -810,6 +814,10 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>_xlfn.STDEV.S(E16:E19)</f>
+        <v>8.1015750803637896E-4</v>
+      </c>
       <c r="E17">
         <f>(H17*9.81*F17^2)/(4*(PI()^2)*G17*I17^2)</f>
         <v>0.17682978186161902</v>
@@ -1056,6 +1064,10 @@
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f>_xlfn.STDEV.S(E23:E30)</f>
+        <v>1.4292774834411627E-4</v>
+      </c>
       <c r="E27">
         <f t="shared" si="5"/>
         <v>2.5112531508388328E-2</v>
@@ -1329,6 +1341,10 @@
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f>_xlfn.STDEV.S(E35:E42)</f>
+        <v>5.274062461195102E-4</v>
+      </c>
       <c r="E39">
         <f t="shared" si="9"/>
         <v>0.16838726694118306</v>

</xml_diff>

<commit_message>
Further along with controller chapter. Only have from tilt angle controller left.
</commit_message>
<xml_diff>
--- a/Design/Mechanical/Inertia Calculation/Bifilar pendulum test 1.xlsx
+++ b/Design/Mechanical/Inertia Calculation/Bifilar pendulum test 1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GusBus\Documents\Masters\Design\Mechanical\Inertia Calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F56EE679-AD9C-430C-A5BB-E6DFC29E6EB4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -436,11 +437,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>